<commit_message>
Pretty sure it works now
</commit_message>
<xml_diff>
--- a/list.xlsx
+++ b/list.xlsx
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2166" uniqueCount="218">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2209" uniqueCount="299">
   <si>
     <t>Sound of Noise</t>
   </si>
@@ -689,6 +689,249 @@
   <si>
     <t>Candy Corn</t>
   </si>
+  <si>
+    <t>Aaron Cadayong</t>
+  </si>
+  <si>
+    <t>Abbey Marye</t>
+  </si>
+  <si>
+    <t>Alex Tan</t>
+  </si>
+  <si>
+    <t>Allison Stevens</t>
+  </si>
+  <si>
+    <t>Anna Raney</t>
+  </si>
+  <si>
+    <t>Anna Stolle</t>
+  </si>
+  <si>
+    <t>Annalise Kendrick</t>
+  </si>
+  <si>
+    <t>Aubri Cisson</t>
+  </si>
+  <si>
+    <t>Austin Albert</t>
+  </si>
+  <si>
+    <t>Austin Schmidt</t>
+  </si>
+  <si>
+    <t>Bethany Mathews</t>
+  </si>
+  <si>
+    <t>Blake Armitage</t>
+  </si>
+  <si>
+    <t>Blake Barger</t>
+  </si>
+  <si>
+    <t>Blake Larson</t>
+  </si>
+  <si>
+    <t>Brandon Widger</t>
+  </si>
+  <si>
+    <t>Briana Andersen</t>
+  </si>
+  <si>
+    <t>BriAnna Martin</t>
+  </si>
+  <si>
+    <t>Brooklyn Cobb</t>
+  </si>
+  <si>
+    <t>Chad McDonald</t>
+  </si>
+  <si>
+    <t>Charlotte Cunningham</t>
+  </si>
+  <si>
+    <t>Christine Hruby</t>
+  </si>
+  <si>
+    <t>Claire Aden</t>
+  </si>
+  <si>
+    <t>Clarisse Eldridge</t>
+  </si>
+  <si>
+    <t>Coby Neumann</t>
+  </si>
+  <si>
+    <t>Cody Hill</t>
+  </si>
+  <si>
+    <t>Cole Elias Reeves</t>
+  </si>
+  <si>
+    <t>Cole Skeffington</t>
+  </si>
+  <si>
+    <t>Devan Bash</t>
+  </si>
+  <si>
+    <t>Devin Clark</t>
+  </si>
+  <si>
+    <t>Diana Boll</t>
+  </si>
+  <si>
+    <t>Elena Guerra</t>
+  </si>
+  <si>
+    <t>Elizabeth Dominic</t>
+  </si>
+  <si>
+    <t>Erik Halsted</t>
+  </si>
+  <si>
+    <t>Henry Ives</t>
+  </si>
+  <si>
+    <t>Hugo Fonck</t>
+  </si>
+  <si>
+    <t>Jacen Hogard</t>
+  </si>
+  <si>
+    <t>Jacob Reed</t>
+  </si>
+  <si>
+    <t>Jesse Hogard</t>
+  </si>
+  <si>
+    <t>Jessi Carman</t>
+  </si>
+  <si>
+    <t>Joey Walker</t>
+  </si>
+  <si>
+    <t>Johnny Dinh</t>
+  </si>
+  <si>
+    <t>Katherine Isabella</t>
+  </si>
+  <si>
+    <t>Katrina Prien</t>
+  </si>
+  <si>
+    <t>Katy Anderson</t>
+  </si>
+  <si>
+    <t>Kaylee Vannice</t>
+  </si>
+  <si>
+    <t>Kurt Sesko</t>
+  </si>
+  <si>
+    <t>Lauren Buckley</t>
+  </si>
+  <si>
+    <t>Lauren Walthall</t>
+  </si>
+  <si>
+    <t>Leonardo Cervera</t>
+  </si>
+  <si>
+    <t>Logan Prieto</t>
+  </si>
+  <si>
+    <t>Mai Jamie</t>
+  </si>
+  <si>
+    <t>Marshall Browne</t>
+  </si>
+  <si>
+    <t>Mary-Ellen Di Giovanni</t>
+  </si>
+  <si>
+    <t>Max Kokosinski</t>
+  </si>
+  <si>
+    <t>Maya Porco</t>
+  </si>
+  <si>
+    <t>Megan Bartlett</t>
+  </si>
+  <si>
+    <t>Mekayla May</t>
+  </si>
+  <si>
+    <t>Michael Jones</t>
+  </si>
+  <si>
+    <t>Natalie Gonzalez</t>
+  </si>
+  <si>
+    <t>Nick Navarro</t>
+  </si>
+  <si>
+    <t>Noah Johnson</t>
+  </si>
+  <si>
+    <t>Olivia Landers</t>
+  </si>
+  <si>
+    <t>Parker Thompson</t>
+  </si>
+  <si>
+    <t>Paul Barker</t>
+  </si>
+  <si>
+    <t>Petra Mannix</t>
+  </si>
+  <si>
+    <t>Reilley Knott</t>
+  </si>
+  <si>
+    <t>Ryan Micheal Crone</t>
+  </si>
+  <si>
+    <t>Ryan Peacock</t>
+  </si>
+  <si>
+    <t>Sadie Smith</t>
+  </si>
+  <si>
+    <t>Sam Mills</t>
+  </si>
+  <si>
+    <t>Samantha Sanson</t>
+  </si>
+  <si>
+    <t>Savanna Elizer</t>
+  </si>
+  <si>
+    <t>Skyler McMullen</t>
+  </si>
+  <si>
+    <t>Sue Steffen</t>
+  </si>
+  <si>
+    <t>Trent Collins</t>
+  </si>
+  <si>
+    <t>Tyler Ennis</t>
+  </si>
+  <si>
+    <t>Tyler Heckenlively</t>
+  </si>
+  <si>
+    <t>Wyatt Kocol</t>
+  </si>
+  <si>
+    <t>Zach Cable</t>
+  </si>
+  <si>
+    <t>Zachary Wall</t>
+  </si>
+  <si>
+    <t>Tim Allcock</t>
+  </si>
 </sst>
 </file>
 
@@ -998,11 +1241,11 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2873,10 +3116,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C38"/>
+  <dimension ref="A1:C81"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:B21"/>
+      <selection sqref="A1:A81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -2885,236 +3128,451 @@
     <col min="3" max="3" width="37.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="46" t="s">
-        <v>0</v>
+    <row r="1" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="44" t="s">
+        <v>218</v>
       </c>
       <c r="B1" s="42"/>
       <c r="C1" s="1"/>
     </row>
     <row r="2" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="46" t="s">
-        <v>3</v>
+      <c r="A2" s="44" t="s">
+        <v>219</v>
       </c>
       <c r="B2" s="43"/>
       <c r="C2" s="1"/>
     </row>
     <row r="3" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="46" t="s">
-        <v>5</v>
+      <c r="A3" s="44" t="s">
+        <v>220</v>
       </c>
       <c r="B3" s="43"/>
       <c r="C3" s="1"/>
     </row>
     <row r="4" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="46" t="s">
-        <v>7</v>
+      <c r="A4" s="44" t="s">
+        <v>221</v>
       </c>
       <c r="B4" s="43"/>
       <c r="C4" s="1"/>
     </row>
     <row r="5" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="46" t="s">
-        <v>8</v>
+      <c r="A5" s="44" t="s">
+        <v>222</v>
       </c>
       <c r="B5" s="43"/>
       <c r="C5" s="1"/>
     </row>
     <row r="6" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="46" t="s">
-        <v>9</v>
+      <c r="A6" s="44" t="s">
+        <v>223</v>
       </c>
       <c r="B6" s="43"/>
       <c r="C6" s="1"/>
     </row>
     <row r="7" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="46" t="s">
-        <v>2</v>
+      <c r="A7" s="44" t="s">
+        <v>224</v>
       </c>
       <c r="B7" s="43"/>
       <c r="C7" s="1"/>
     </row>
     <row r="8" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="46" t="s">
-        <v>4</v>
+      <c r="A8" s="44" t="s">
+        <v>225</v>
       </c>
       <c r="B8" s="43"/>
       <c r="C8" s="1"/>
     </row>
     <row r="9" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="46" t="s">
-        <v>6</v>
+      <c r="A9" s="44" t="s">
+        <v>226</v>
       </c>
       <c r="B9" s="43"/>
       <c r="C9" s="1"/>
     </row>
     <row r="10" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="46" t="s">
-        <v>10</v>
+      <c r="A10" s="44" t="s">
+        <v>227</v>
       </c>
       <c r="B10" s="43"/>
       <c r="C10" s="1"/>
     </row>
     <row r="11" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="46" t="s">
-        <v>11</v>
+      <c r="A11" s="44" t="s">
+        <v>228</v>
       </c>
       <c r="B11" s="43"/>
       <c r="C11" s="1"/>
     </row>
     <row r="12" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="46" t="s">
-        <v>13</v>
+      <c r="A12" s="44" t="s">
+        <v>229</v>
       </c>
       <c r="B12" s="43"/>
       <c r="C12" s="1"/>
     </row>
     <row r="13" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="46" t="s">
-        <v>12</v>
+      <c r="A13" s="44" t="s">
+        <v>230</v>
       </c>
       <c r="B13" s="43"/>
       <c r="C13" s="1"/>
     </row>
     <row r="14" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="46" t="s">
-        <v>16</v>
+      <c r="A14" s="44" t="s">
+        <v>231</v>
       </c>
       <c r="B14" s="43"/>
       <c r="C14" s="1"/>
     </row>
     <row r="15" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="46" t="s">
-        <v>18</v>
+      <c r="A15" s="44" t="s">
+        <v>232</v>
       </c>
       <c r="B15" s="43"/>
       <c r="C15" s="1"/>
     </row>
     <row r="16" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="46" t="s">
-        <v>19</v>
+      <c r="A16" s="44" t="s">
+        <v>233</v>
       </c>
       <c r="B16" s="43"/>
       <c r="C16" s="1"/>
     </row>
     <row r="17" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="46" t="s">
-        <v>14</v>
+      <c r="A17" s="44" t="s">
+        <v>234</v>
       </c>
       <c r="B17" s="43"/>
       <c r="C17" s="1"/>
     </row>
     <row r="18" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="46" t="s">
-        <v>15</v>
+      <c r="A18" s="44" t="s">
+        <v>235</v>
       </c>
       <c r="B18" s="43"/>
       <c r="C18" s="1"/>
     </row>
     <row r="19" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="46" t="s">
-        <v>20</v>
+      <c r="A19" s="44" t="s">
+        <v>236</v>
       </c>
       <c r="B19" s="43"/>
       <c r="C19" s="1"/>
     </row>
     <row r="20" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="46" t="s">
-        <v>17</v>
+      <c r="A20" s="44" t="s">
+        <v>237</v>
       </c>
       <c r="B20" s="43"/>
       <c r="C20" s="1"/>
     </row>
     <row r="21" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="46" t="s">
-        <v>23</v>
+      <c r="A21" s="44" t="s">
+        <v>238</v>
       </c>
       <c r="B21" s="43"/>
       <c r="C21" s="1"/>
     </row>
     <row r="22" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="46" t="s">
-        <v>24</v>
+      <c r="A22" s="44" t="s">
+        <v>239</v>
       </c>
     </row>
     <row r="23" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="46" t="s">
-        <v>21</v>
+      <c r="A23" s="44" t="s">
+        <v>240</v>
       </c>
     </row>
     <row r="24" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="46" t="s">
-        <v>27</v>
+      <c r="A24" s="44" t="s">
+        <v>241</v>
       </c>
     </row>
     <row r="25" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="46" t="s">
-        <v>29</v>
+      <c r="A25" s="44" t="s">
+        <v>242</v>
       </c>
     </row>
     <row r="26" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="46" t="s">
-        <v>25</v>
+      <c r="A26" s="44" t="s">
+        <v>243</v>
       </c>
     </row>
     <row r="27" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="46" t="s">
-        <v>22</v>
+      <c r="A27" s="44" t="s">
+        <v>244</v>
       </c>
     </row>
     <row r="28" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="46" t="s">
-        <v>30</v>
+      <c r="A28" s="44" t="s">
+        <v>245</v>
       </c>
     </row>
     <row r="29" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="46" t="s">
-        <v>31</v>
+      <c r="A29" s="44" t="s">
+        <v>246</v>
       </c>
     </row>
     <row r="30" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="46" t="s">
-        <v>28</v>
+      <c r="A30" s="44" t="s">
+        <v>247</v>
       </c>
     </row>
     <row r="31" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="46" t="s">
-        <v>33</v>
+      <c r="A31" s="44" t="s">
+        <v>248</v>
       </c>
     </row>
     <row r="32" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="46" t="s">
-        <v>35</v>
+      <c r="A32" s="44" t="s">
+        <v>249</v>
       </c>
     </row>
     <row r="33" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="46" t="s">
-        <v>26</v>
+      <c r="A33" s="44" t="s">
+        <v>250</v>
       </c>
     </row>
     <row r="34" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="46" t="s">
-        <v>34</v>
+      <c r="A34" s="44" t="s">
+        <v>251</v>
       </c>
     </row>
     <row r="35" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="46" t="s">
-        <v>37</v>
+      <c r="A35" s="44" t="s">
+        <v>252</v>
       </c>
     </row>
     <row r="36" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="46" t="s">
-        <v>38</v>
+      <c r="A36" s="44" t="s">
+        <v>253</v>
       </c>
     </row>
     <row r="37" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="46" t="s">
-        <v>32</v>
+      <c r="A37" s="44" t="s">
+        <v>254</v>
       </c>
     </row>
     <row r="38" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="46" t="s">
-        <v>36</v>
+      <c r="A38" s="44" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A39" s="44" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A40" s="44" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A41" s="44" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A42" s="44" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A43" s="44" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A44" s="44" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A45" s="44" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="46" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A46" s="44" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A47" s="44" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="48" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A48" s="44" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A49" s="44" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A50" s="44" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A51" s="44" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="52" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A52" s="44" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="53" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A53" s="44" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="54" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A54" s="44" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="55" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A55" s="44" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="56" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A56" s="44" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="57" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A57" s="44" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="58" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A58" s="44" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="59" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A59" s="44" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="60" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A60" s="44" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="61" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A61" s="44" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="62" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A62" s="44" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="63" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A63" s="44" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="64" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A64" s="44" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="65" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A65" s="44" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="66" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A66" s="44" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="67" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A67" s="44" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="68" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A68" s="44" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="69" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A69" s="44" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="70" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A70" s="44" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="71" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A71" s="44" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="72" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A72" s="44" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="73" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A73" s="44" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="74" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A74" s="44" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="75" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A75" s="44" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="76" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A76" s="44" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="77" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A77" s="44" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="78" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A78" s="44" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="79" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A79" s="44" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="80" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A80" s="44" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="81" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A81" s="44" t="s">
+        <v>298</v>
       </c>
     </row>
   </sheetData>
@@ -3138,7 +3596,7 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="44" t="s">
+      <c r="B1" s="45" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
@@ -3149,7 +3607,7 @@
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="45"/>
+      <c r="B2" s="46"/>
       <c r="C2" s="1" t="s">
         <v>4</v>
       </c>
@@ -3158,7 +3616,7 @@
       <c r="A3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="45"/>
+      <c r="B3" s="46"/>
       <c r="C3" s="1" t="s">
         <v>6</v>
       </c>
@@ -3167,7 +3625,7 @@
       <c r="A4" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="45"/>
+      <c r="B4" s="46"/>
       <c r="C4" s="1" t="s">
         <v>0</v>
       </c>
@@ -3176,7 +3634,7 @@
       <c r="A5" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="45"/>
+      <c r="B5" s="46"/>
       <c r="C5" s="1" t="s">
         <v>3</v>
       </c>
@@ -3185,7 +3643,7 @@
       <c r="A6" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B6" s="45"/>
+      <c r="B6" s="46"/>
       <c r="C6" s="1" t="s">
         <v>8</v>
       </c>
@@ -3194,7 +3652,7 @@
       <c r="A7" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B7" s="45"/>
+      <c r="B7" s="46"/>
       <c r="C7" s="1" t="s">
         <v>5</v>
       </c>
@@ -3203,7 +3661,7 @@
       <c r="A8" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B8" s="45"/>
+      <c r="B8" s="46"/>
       <c r="C8" s="1" t="s">
         <v>7</v>
       </c>
@@ -3212,7 +3670,7 @@
       <c r="A9" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B9" s="45"/>
+      <c r="B9" s="46"/>
       <c r="C9" s="1" t="s">
         <v>10</v>
       </c>
@@ -3221,7 +3679,7 @@
       <c r="A10" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B10" s="45"/>
+      <c r="B10" s="46"/>
       <c r="C10" s="1" t="s">
         <v>11</v>
       </c>
@@ -3230,7 +3688,7 @@
       <c r="A11" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B11" s="45"/>
+      <c r="B11" s="46"/>
       <c r="C11" s="1" t="s">
         <v>12</v>
       </c>
@@ -3239,7 +3697,7 @@
       <c r="A12" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B12" s="45"/>
+      <c r="B12" s="46"/>
       <c r="C12" s="1" t="s">
         <v>14</v>
       </c>
@@ -3248,7 +3706,7 @@
       <c r="A13" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B13" s="45"/>
+      <c r="B13" s="46"/>
       <c r="C13" s="1" t="s">
         <v>15</v>
       </c>
@@ -3257,7 +3715,7 @@
       <c r="A14" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B14" s="45"/>
+      <c r="B14" s="46"/>
       <c r="C14" s="1" t="s">
         <v>17</v>
       </c>
@@ -3266,7 +3724,7 @@
       <c r="A15" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B15" s="45"/>
+      <c r="B15" s="46"/>
       <c r="C15" s="1" t="s">
         <v>19</v>
       </c>
@@ -3275,7 +3733,7 @@
       <c r="A16" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B16" s="45"/>
+      <c r="B16" s="46"/>
       <c r="C16" s="1" t="s">
         <v>9</v>
       </c>
@@ -3284,7 +3742,7 @@
       <c r="A17" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B17" s="45"/>
+      <c r="B17" s="46"/>
       <c r="C17" s="1" t="s">
         <v>18</v>
       </c>
@@ -3293,7 +3751,7 @@
       <c r="A18" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B18" s="45"/>
+      <c r="B18" s="46"/>
       <c r="C18" s="1" t="s">
         <v>16</v>
       </c>
@@ -3302,7 +3760,7 @@
       <c r="A19" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B19" s="45"/>
+      <c r="B19" s="46"/>
       <c r="C19" s="1" t="s">
         <v>21</v>
       </c>
@@ -3311,7 +3769,7 @@
       <c r="A20" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B20" s="45"/>
+      <c r="B20" s="46"/>
       <c r="C20" s="1" t="s">
         <v>22</v>
       </c>
@@ -3320,7 +3778,7 @@
       <c r="A21" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B21" s="45"/>
+      <c r="B21" s="46"/>
       <c r="C21" s="1" t="s">
         <v>23</v>
       </c>
@@ -3329,7 +3787,7 @@
       <c r="A22" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B22" s="45"/>
+      <c r="B22" s="46"/>
       <c r="C22" s="1" t="s">
         <v>25</v>
       </c>
@@ -3338,7 +3796,7 @@
       <c r="A23" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B23" s="45"/>
+      <c r="B23" s="46"/>
       <c r="C23" s="1" t="s">
         <v>26</v>
       </c>
@@ -3347,7 +3805,7 @@
       <c r="A24" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B24" s="45"/>
+      <c r="B24" s="46"/>
       <c r="C24" s="1" t="s">
         <v>28</v>
       </c>
@@ -3356,7 +3814,7 @@
       <c r="A25" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B25" s="45"/>
+      <c r="B25" s="46"/>
       <c r="C25" s="1" t="s">
         <v>29</v>
       </c>
@@ -3365,7 +3823,7 @@
       <c r="A26" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B26" s="45"/>
+      <c r="B26" s="46"/>
       <c r="C26" s="1" t="s">
         <v>27</v>
       </c>
@@ -3374,7 +3832,7 @@
       <c r="A27" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B27" s="45"/>
+      <c r="B27" s="46"/>
       <c r="C27" s="1" t="s">
         <v>30</v>
       </c>
@@ -3383,7 +3841,7 @@
       <c r="A28" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="B28" s="45"/>
+      <c r="B28" s="46"/>
       <c r="C28" s="1" t="s">
         <v>13</v>
       </c>
@@ -3392,7 +3850,7 @@
       <c r="A29" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="B29" s="45"/>
+      <c r="B29" s="46"/>
       <c r="C29" s="1" t="s">
         <v>20</v>
       </c>
@@ -3401,7 +3859,7 @@
       <c r="A30" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B30" s="45"/>
+      <c r="B30" s="46"/>
       <c r="C30" s="1" t="s">
         <v>32</v>
       </c>
@@ -3410,7 +3868,7 @@
       <c r="A31" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="B31" s="45"/>
+      <c r="B31" s="46"/>
       <c r="C31" s="1" t="s">
         <v>34</v>
       </c>
@@ -3419,7 +3877,7 @@
       <c r="A32" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="B32" s="45"/>
+      <c r="B32" s="46"/>
       <c r="C32" s="1" t="s">
         <v>36</v>
       </c>
@@ -3428,7 +3886,7 @@
       <c r="A33" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B33" s="45"/>
+      <c r="B33" s="46"/>
       <c r="C33" s="1" t="s">
         <v>24</v>
       </c>
@@ -3437,7 +3895,7 @@
       <c r="A34" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B34" s="45"/>
+      <c r="B34" s="46"/>
       <c r="C34" s="1" t="s">
         <v>33</v>
       </c>
@@ -3446,7 +3904,7 @@
       <c r="A35" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="B35" s="45"/>
+      <c r="B35" s="46"/>
       <c r="C35" s="1" t="s">
         <v>35</v>
       </c>
@@ -3455,7 +3913,7 @@
       <c r="A36" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="B36" s="45"/>
+      <c r="B36" s="46"/>
       <c r="C36" s="1" t="s">
         <v>31</v>
       </c>
@@ -3464,7 +3922,7 @@
       <c r="A37" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="B37" s="45"/>
+      <c r="B37" s="46"/>
       <c r="C37" s="1" t="s">
         <v>37</v>
       </c>
@@ -3473,7 +3931,7 @@
       <c r="A38" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="B38" s="45"/>
+      <c r="B38" s="46"/>
       <c r="C38" s="1" t="s">
         <v>38</v>
       </c>

</xml_diff>